<commit_message>
load graph & papers
</commit_message>
<xml_diff>
--- a/test_suite.xlsx
+++ b/test_suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanachilukuri/Documents/GitHub/bayou_mcmc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BCD2FB-B3BB-8D40-BEB5-04DD6A34E688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF99E9-B1DB-9646-9ED6-B31D10EE2A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19360" xr2:uid="{3748C879-CD03-2749-8951-9D666A6F63D9}"/>
   </bookViews>
@@ -3616,7 +3616,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>